<commit_message>
Clean up output width and height for convolutions
</commit_message>
<xml_diff>
--- a/results/inference/device/DeepBench_Raspberry_Pi_3.xlsx
+++ b/results/inference/device/DeepBench_Raspberry_Pi_3.xlsx
@@ -686,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q64"/>
+  <dimension ref="A1:S64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1087,7 +1087,7 @@
         <v>0.52211095553087739</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:19">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1099,7 +1099,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:19">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1111,7 +1111,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:19">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1123,7 +1123,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:19">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:19">
       <c r="B21" s="1"/>
       <c r="C21">
         <v>7680</v>
@@ -1194,7 +1194,7 @@
         <v>1.8246008279124777</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:19">
       <c r="B22" s="1"/>
       <c r="C22">
         <v>7680</v>
@@ -1230,7 +1230,7 @@
         <v>6.1237807052188549</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:19">
       <c r="B23" s="1"/>
       <c r="C23">
         <v>10752</v>
@@ -1266,7 +1266,7 @@
         <v>1.8237277928334839</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:19">
       <c r="B24" s="1"/>
       <c r="C24">
         <v>10752</v>
@@ -1302,7 +1302,7 @@
         <v>6.119149895770553</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:19">
       <c r="B25" s="1"/>
       <c r="C25">
         <v>7680</v>
@@ -1338,7 +1338,7 @@
         <v>0.92824923317495645</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:19">
       <c r="B26" s="1"/>
       <c r="C26">
         <v>7680</v>
@@ -1373,8 +1373,12 @@
         <f t="shared" si="2"/>
         <v>3.1264453102230148</v>
       </c>
-    </row>
-    <row r="27" spans="1:17">
+      <c r="S26">
+        <f>ROUNDDOWN(1.6,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
       <c r="B27" s="1"/>
       <c r="C27">
         <v>10752</v>
@@ -1410,7 +1414,7 @@
         <v>0.92516612814729016</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:19">
       <c r="B28" s="1"/>
       <c r="C28">
         <v>10752</v>
@@ -1446,10 +1450,10 @@
         <v>3.1022798750891694</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:19">
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:19">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1461,12 +1465,12 @@
       <c r="I30" s="1"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:19">
       <c r="A31" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:19">
       <c r="C32" t="s">
         <v>15</v>
       </c>
@@ -1551,15 +1555,15 @@
         <v>35</v>
       </c>
       <c r="O33" s="2">
-        <f>(C33-H33+1+2*K33)/L33</f>
-        <v>18.5</v>
+        <f>1+ROUNDDOWN((($C33-$H33+2*$J33)/$L33),0)</f>
+        <v>19</v>
       </c>
       <c r="P33" s="2">
-        <f>(D33-I33+1+2*J33)/M33</f>
+        <f>1+ROUNDDOWN((($D33-$I33+2*$K33)/$M33),0)</f>
         <v>26</v>
       </c>
       <c r="Q33" s="3" t="e">
-        <f>(2*O33*P33*F33*G33*E33*I33*H33)/(N33/1000)/10^9</f>
+        <f t="shared" ref="Q33:Q49" si="3">(2*O33*P33*F33*G33*E33*I33*H33)/(N33/1000)/10^9</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1603,15 +1607,15 @@
         <v>670.75300000000004</v>
       </c>
       <c r="O34" s="2">
-        <f>(C34-H34+1+2*K34)/L34</f>
+        <f t="shared" ref="O34:O49" si="4">1+ROUNDDOWN((($C34-$H34+2*$J34)/$L34),0)</f>
         <v>112</v>
       </c>
       <c r="P34" s="2">
-        <f>(D34-I34+1+2*J34)/M34</f>
+        <f t="shared" ref="P34:P49" si="5">1+ROUNDDOWN((($D34-$I34+2*$K34)/$M34),0)</f>
         <v>112</v>
       </c>
       <c r="Q34" s="3">
-        <f>(2*O34*P34*F34*G34*E34*I34*H34)/(N34/1000)/10^9</f>
+        <f t="shared" si="3"/>
         <v>0.15320162265394263</v>
       </c>
     </row>
@@ -1655,15 +1659,15 @@
         <v>601.14700000000005</v>
       </c>
       <c r="O35" s="2">
-        <f>(C35-H35+1+2*K35)/L35</f>
+        <f t="shared" si="4"/>
         <v>56</v>
       </c>
       <c r="P35" s="2">
-        <f>(D35-I35+1+2*J35)/M35</f>
+        <f t="shared" si="5"/>
         <v>56</v>
       </c>
       <c r="Q35" s="3">
-        <f>(2*O35*P35*F35*G35*E35*I35*H35)/(N35/1000)/10^9</f>
+        <f t="shared" si="3"/>
         <v>0.17094063182549357</v>
       </c>
     </row>
@@ -1707,15 +1711,15 @@
         <v>577.96799999999996</v>
       </c>
       <c r="O36" s="2">
-        <f>(C36-H36+1+2*K36)/L36</f>
+        <f t="shared" si="4"/>
         <v>56</v>
       </c>
       <c r="P36" s="2">
-        <f>(D36-I36+1+2*J36)/M36</f>
+        <f t="shared" si="5"/>
         <v>56</v>
       </c>
       <c r="Q36" s="3">
-        <f>(2*O36*P36*F36*G36*E36*I36*H36)/(N36/1000)/10^9</f>
+        <f t="shared" si="3"/>
         <v>0.17779608559643442</v>
       </c>
     </row>
@@ -1759,15 +1763,15 @@
         <v>185.87200000000001</v>
       </c>
       <c r="O37" s="2">
-        <f>(C37-H37+1+2*K37)/L37</f>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="P37" s="2">
-        <f>(D37-I37+1+2*J37)/M37</f>
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="Q37" s="3">
-        <f>(2*O37*P37*F37*G37*E37*I37*H37)/(N37/1000)/10^9</f>
+        <f t="shared" si="3"/>
         <v>0.27642799345786345</v>
       </c>
     </row>
@@ -1811,15 +1815,15 @@
         <v>557.25599999999997</v>
       </c>
       <c r="O38" s="2">
-        <f>(C38-H38+1+2*K38)/L38</f>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="P38" s="2">
-        <f>(D38-I38+1+2*J38)/M38</f>
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="Q38" s="3">
-        <f>(2*O38*P38*F38*G38*E38*I38*H38)/(N38/1000)/10^9</f>
+        <f t="shared" si="3"/>
         <v>0.1844043814691991</v>
       </c>
     </row>
@@ -1863,15 +1867,15 @@
         <v>391.67899999999997</v>
       </c>
       <c r="O39" s="2">
-        <f>(C39-H39+1+2*K39)/L39</f>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="P39" s="2">
-        <f>(D39-I39+1+2*J39)/M39</f>
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="Q39" s="3">
-        <f>(2*O39*P39*F39*G39*E39*I39*H39)/(N39/1000)/10^9</f>
+        <f t="shared" si="3"/>
         <v>0.26235883976419466</v>
       </c>
     </row>
@@ -1915,15 +1919,15 @@
         <v>168.21700000000001</v>
       </c>
       <c r="O40" s="2">
-        <f>(C40-H40+1+2*K40)/L40</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="P40" s="2">
-        <f>(D40-I40+1+2*J40)/M40</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="Q40" s="3">
-        <f>(2*O40*P40*F40*G40*E40*I40*H40)/(N40/1000)/10^9</f>
+        <f t="shared" si="3"/>
         <v>0.30544013981939994</v>
       </c>
     </row>
@@ -1967,15 +1971,15 @@
         <v>633.46799999999996</v>
       </c>
       <c r="O41" s="2">
-        <f>(C41-H41+1+2*K41)/L41</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="P41" s="2">
-        <f>(D41-I41+1+2*J41)/M41</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="Q41" s="3">
-        <f>(2*O41*P41*F41*G41*E41*I41*H41)/(N41/1000)/10^9</f>
+        <f t="shared" si="3"/>
         <v>0.16221884609798759</v>
       </c>
     </row>
@@ -2019,15 +2023,15 @@
         <v>1258.2650000000001</v>
       </c>
       <c r="O42" s="2">
-        <f>(C42-H42+1+2*K42)/L42</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="P42" s="2">
-        <f>(D42-I42+1+2*J42)/M42</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="Q42" s="3">
-        <f>(2*O42*P42*F42*G42*E42*I42*H42)/(N42/1000)/10^9</f>
+        <f t="shared" si="3"/>
         <v>0.16333673431272422</v>
       </c>
     </row>
@@ -2071,15 +2075,15 @@
         <v>344.66800000000001</v>
       </c>
       <c r="O43" s="2">
-        <f>(C43-H43+1+2*K43)/L43</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="P43" s="2">
-        <f>(D43-I43+1+2*J43)/M43</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="Q43" s="3">
-        <f>(2*O43*P43*F43*G43*E43*I43*H43)/(N43/1000)/10^9</f>
+        <f t="shared" si="3"/>
         <v>0.29814327990994227</v>
       </c>
     </row>
@@ -2123,15 +2127,15 @@
         <v>652.13099999999997</v>
       </c>
       <c r="O44" s="2">
-        <f>(C44-H44+1+2*K44)/L44</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="P44" s="2">
-        <f>(D44-I44+1+2*J44)/M44</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="Q44" s="3">
-        <f>(2*O44*P44*F44*G44*E44*I44*H44)/(N44/1000)/10^9</f>
+        <f t="shared" si="3"/>
         <v>0.15757638879304925</v>
       </c>
     </row>
@@ -2175,15 +2179,15 @@
         <v>278.46800000000002</v>
       </c>
       <c r="O45" s="2">
-        <f>(C45-H45+1+2*K45)/L45</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="P45" s="2">
-        <f>(D45-I45+1+2*J45)/M45</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="Q45" s="3">
-        <f>(2*O45*P45*F45*G45*E45*I45*H45)/(N45/1000)/10^9</f>
+        <f t="shared" si="3"/>
         <v>0.18451033511929557</v>
       </c>
     </row>
@@ -2227,15 +2231,15 @@
         <v>149.422</v>
       </c>
       <c r="O46" s="2">
-        <f>(C46-H46+1+2*K46)/L46</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="P46" s="2">
-        <f>(D46-I46+1+2*J46)/M46</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="Q46" s="3">
-        <f>(2*O46*P46*F46*G46*E46*I46*H46)/(N46/1000)/10^9</f>
+        <f t="shared" si="3"/>
         <v>1.5473692495081046</v>
       </c>
     </row>
@@ -2279,15 +2283,15 @@
         <v>735.28200000000004</v>
       </c>
       <c r="O47" s="2">
-        <f>(C47-H47+1+2*K47)/L47</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="P47" s="2">
-        <f>(D47-I47+1+2*J47)/M47</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="Q47" s="3">
-        <f>(2*O47*P47*F47*G47*E47*I47*H47)/(N47/1000)/10^9</f>
+        <f t="shared" si="3"/>
         <v>0.13975651246732546</v>
       </c>
     </row>
@@ -2331,15 +2335,15 @@
         <v>1498.7280000000001</v>
       </c>
       <c r="O48" s="2">
-        <f>(C48-H48+1+2*K48)/L48</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="P48" s="2">
-        <f>(D48-I48+1+2*J48)/M48</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="Q48" s="3">
-        <f>(2*O48*P48*F48*G48*E48*I48*H48)/(N48/1000)/10^9</f>
+        <f t="shared" si="3"/>
         <v>0.13713021709075965</v>
       </c>
     </row>
@@ -2383,15 +2387,15 @@
         <v>563.92899999999997</v>
       </c>
       <c r="O49" s="2">
-        <f>(C49-H49+1+2*K49)/L49</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="P49" s="2">
-        <f>(D49-I49+1+2*J49)/M49</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="Q49" s="3">
-        <f>(2*O49*P49*F49*G49*E49*I49*H49)/(N49/1000)/10^9</f>
+        <f t="shared" si="3"/>
         <v>0.18222231522053306</v>
       </c>
     </row>

</xml_diff>